<commit_message>
Central fed. dist. 13-14 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/cities13-14/0/d1.xlsx
+++ b/migforecasting/cities13-14/0/d1.xlsx
@@ -3326,8 +3326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,12 +3396,8 @@
       <c r="V1" s="1">
         <v>20</v>
       </c>
-      <c r="W1" s="1">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1">
-        <v>22</v>
-      </c>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -8034,9 +8030,7 @@
       </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
-        <v>77</v>
-      </c>
+      <c r="A79" s="1"/>
       <c r="B79" t="s">
         <v>958</v>
       </c>

</xml_diff>